<commit_message>
Fixed 004, todo - solve issue with saver functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/shipping-table.xlsx
+++ b/src/main/resources/templates/shipping-table.xlsx
@@ -1584,7 +1584,7 @@
     <t xml:space="preserve">С-1-46</t>
   </si>
   <si>
-    <t xml:space="preserve">  СМК-20034-КМД</t>
+    <t xml:space="preserve">СМК-20034-КМД</t>
   </si>
   <si>
     <t xml:space="preserve">ЖД Пристройка к производственному цеху в муниципии Кишинеу  на улице Мунчешть 801  отгрузка</t>
@@ -2964,7 +2964,7 @@
     <t xml:space="preserve">Ж-148</t>
   </si>
   <si>
-    <t xml:space="preserve">  СМК-20036-КМД</t>
+    <t xml:space="preserve">СМК-20036-КМД</t>
   </si>
   <si>
     <t xml:space="preserve">ВС1-1</t>
@@ -15989,9 +15989,9 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A648" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A747" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C655" activeCellId="0" sqref="C655"/>
+      <selection pane="bottomLeft" activeCell="C706" activeCellId="0" sqref="C706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>